<commit_message>
rr_templates.xlsx now has crossover rr formats
</commit_message>
<xml_diff>
--- a/templates/rr_schedules/rr_templates.xlsx
+++ b/templates/rr_schedules/rr_templates.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\z004ercu\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B0E66BC-2560-4C19-8F12-5C327E14DA07}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE4E61D5-8EBD-4394-BDA9-45302CD3B0B3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="57490" yWindow="-110" windowWidth="29020" windowHeight="15820" xr2:uid="{9E58356C-D73F-FC43-AA9C-FFAB6CC6AEB1}"/>
+    <workbookView xWindow="28690" yWindow="-110" windowWidth="29020" windowHeight="15820" activeTab="12" xr2:uid="{9E58356C-D73F-FC43-AA9C-FFAB6CC6AEB1}"/>
   </bookViews>
   <sheets>
     <sheet name="rr_3" sheetId="12" r:id="rId1"/>
@@ -25,6 +25,12 @@
     <sheet name="rr_12" sheetId="5" r:id="rId10"/>
     <sheet name="rr_13" sheetId="3" r:id="rId11"/>
     <sheet name="rr_14" sheetId="4" r:id="rId12"/>
+    <sheet name="rr_crossover_B3" sheetId="13" r:id="rId13"/>
+    <sheet name="rr_crossover_A6" sheetId="14" r:id="rId14"/>
+    <sheet name="rr_crossover_B6" sheetId="15" r:id="rId15"/>
+    <sheet name="rr_crossover_B7" sheetId="16" r:id="rId16"/>
+    <sheet name="rr_crossover_A8" sheetId="17" r:id="rId17"/>
+    <sheet name="rr_crossover_B8" sheetId="18" r:id="rId18"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -42,9 +48,56 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="14">
+  <si>
+    <t>A1</t>
+  </si>
+  <si>
+    <t>B2</t>
+  </si>
+  <si>
+    <t>C1</t>
+  </si>
+  <si>
+    <t>D2</t>
+  </si>
+  <si>
+    <t>B1</t>
+  </si>
+  <si>
+    <t>A2</t>
+  </si>
+  <si>
+    <t>D1</t>
+  </si>
+  <si>
+    <t>C2</t>
+  </si>
+  <si>
+    <t>round 1</t>
+  </si>
+  <si>
+    <t>round 2</t>
+  </si>
+  <si>
+    <t>round 3</t>
+  </si>
+  <si>
+    <t>round 4</t>
+  </si>
+  <si>
+    <t>round 5</t>
+  </si>
+  <si>
+    <t>round 6</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5">
+  <fonts count="7">
     <font>
       <sz val="16"/>
       <color theme="1"/>
@@ -75,6 +128,17 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -96,7 +160,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -116,6 +180,10 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -433,7 +501,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{17D1A3EF-1D2C-9645-AE2E-821B882D0ED5}">
   <dimension ref="A2:C4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
@@ -2041,6 +2109,819 @@
       </c>
       <c r="N14" s="2">
         <v>11</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{79C39426-53E4-4FE4-BE56-C0D0A1CEAC29}">
+  <dimension ref="A2:C4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="20"/>
+  <sheetData>
+    <row r="2" spans="1:3">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>2</v>
+      </c>
+      <c r="C2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3">
+        <v>3</v>
+      </c>
+      <c r="C3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4">
+        <v>2</v>
+      </c>
+      <c r="C4">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6ACCB1AB-6FF2-4899-B7EC-146C060423D8}">
+  <dimension ref="A2:F4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:C4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="20"/>
+  <sheetData>
+    <row r="2" spans="1:6">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>6</v>
+      </c>
+      <c r="C2">
+        <v>3</v>
+      </c>
+      <c r="D2">
+        <v>4</v>
+      </c>
+      <c r="E2">
+        <v>2</v>
+      </c>
+      <c r="F2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3">
+        <v>3</v>
+      </c>
+      <c r="C3">
+        <v>5</v>
+      </c>
+      <c r="D3">
+        <v>6</v>
+      </c>
+      <c r="E3">
+        <v>1</v>
+      </c>
+      <c r="F3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
+      <c r="A4">
+        <v>4</v>
+      </c>
+      <c r="B4">
+        <v>5</v>
+      </c>
+      <c r="C4">
+        <v>1</v>
+      </c>
+      <c r="D4">
+        <v>2</v>
+      </c>
+      <c r="E4">
+        <v>3</v>
+      </c>
+      <c r="F4">
+        <v>6</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{77A22584-AFAA-4FEB-B469-5327230FF0CE}">
+  <dimension ref="A2:F5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:C4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="20"/>
+  <sheetData>
+    <row r="2" spans="1:6">
+      <c r="A2">
+        <v>5</v>
+      </c>
+      <c r="B2">
+        <v>4</v>
+      </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
+      <c r="D2">
+        <v>6</v>
+      </c>
+      <c r="E2">
+        <v>3</v>
+      </c>
+      <c r="F2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3">
+        <v>6</v>
+      </c>
+      <c r="C3">
+        <v>3</v>
+      </c>
+      <c r="D3">
+        <v>5</v>
+      </c>
+      <c r="E3">
+        <v>1</v>
+      </c>
+      <c r="F3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4">
+        <v>6</v>
+      </c>
+      <c r="C4">
+        <v>2</v>
+      </c>
+      <c r="D4">
+        <v>4</v>
+      </c>
+      <c r="E4">
+        <v>1</v>
+      </c>
+      <c r="F4">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
+      <c r="A5">
+        <v>1</v>
+      </c>
+      <c r="B5">
+        <v>3</v>
+      </c>
+      <c r="C5">
+        <v>5</v>
+      </c>
+      <c r="D5">
+        <v>2</v>
+      </c>
+      <c r="E5">
+        <v>4</v>
+      </c>
+      <c r="F5">
+        <v>6</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{32003450-3219-48C1-9C9F-E5D29053980A}">
+  <dimension ref="A2:J21"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:C4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="10.77734375" defaultRowHeight="23"/>
+  <cols>
+    <col min="1" max="16384" width="10.77734375" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:10">
+      <c r="A2" s="1">
+        <v>5</v>
+      </c>
+      <c r="B2" s="1">
+        <v>6</v>
+      </c>
+      <c r="C2" s="1">
+        <v>2</v>
+      </c>
+      <c r="D2" s="1">
+        <v>5</v>
+      </c>
+      <c r="E2" s="1">
+        <v>4</v>
+      </c>
+      <c r="F2" s="1">
+        <v>7</v>
+      </c>
+      <c r="G2" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10">
+      <c r="A3" s="1">
+        <v>3</v>
+      </c>
+      <c r="B3" s="1">
+        <v>5</v>
+      </c>
+      <c r="C3" s="1">
+        <v>4</v>
+      </c>
+      <c r="D3" s="1">
+        <v>6</v>
+      </c>
+      <c r="E3" s="1">
+        <v>5</v>
+      </c>
+      <c r="F3" s="1">
+        <v>7</v>
+      </c>
+      <c r="G3" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10">
+      <c r="A4" s="1">
+        <v>2</v>
+      </c>
+      <c r="B4" s="1">
+        <v>7</v>
+      </c>
+      <c r="C4" s="1">
+        <v>3</v>
+      </c>
+      <c r="D4" s="1">
+        <v>6</v>
+      </c>
+      <c r="E4" s="1">
+        <v>4</v>
+      </c>
+      <c r="F4" s="1">
+        <v>5</v>
+      </c>
+      <c r="G4" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10">
+      <c r="A5" s="1">
+        <v>6</v>
+      </c>
+      <c r="B5" s="1">
+        <v>7</v>
+      </c>
+      <c r="C5" s="1">
+        <v>5</v>
+      </c>
+      <c r="D5" s="1">
+        <v>4</v>
+      </c>
+      <c r="E5" s="1">
+        <v>2</v>
+      </c>
+      <c r="F5" s="1">
+        <v>3</v>
+      </c>
+      <c r="G5" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10">
+      <c r="A6" s="1">
+        <v>2</v>
+      </c>
+      <c r="B6" s="1">
+        <v>4</v>
+      </c>
+      <c r="C6" s="1">
+        <v>5</v>
+      </c>
+      <c r="D6" s="1">
+        <v>7</v>
+      </c>
+      <c r="E6" s="1">
+        <v>5</v>
+      </c>
+      <c r="F6" s="1">
+        <v>3</v>
+      </c>
+      <c r="G6" s="1">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10">
+      <c r="A7" s="1">
+        <v>3</v>
+      </c>
+      <c r="B7" s="1">
+        <v>4</v>
+      </c>
+      <c r="C7" s="1">
+        <v>5</v>
+      </c>
+      <c r="D7" s="1">
+        <v>2</v>
+      </c>
+      <c r="E7" s="1">
+        <v>5</v>
+      </c>
+      <c r="F7" s="1">
+        <v>6</v>
+      </c>
+      <c r="G7" s="1">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10">
+      <c r="B10" s="10"/>
+      <c r="D10" s="10"/>
+      <c r="F10" s="10"/>
+      <c r="H10" s="10"/>
+    </row>
+    <row r="11" spans="1:10">
+      <c r="A11" s="10"/>
+      <c r="B11" s="10"/>
+      <c r="D11" s="10"/>
+      <c r="F11" s="10"/>
+      <c r="H11" s="10"/>
+    </row>
+    <row r="12" spans="1:10">
+      <c r="A12" s="10"/>
+      <c r="B12" s="10"/>
+      <c r="D12" s="10"/>
+      <c r="F12" s="10"/>
+      <c r="H12" s="10"/>
+    </row>
+    <row r="13" spans="1:10">
+      <c r="A13" s="10"/>
+      <c r="B13" s="10"/>
+      <c r="D13" s="10"/>
+      <c r="F13" s="10"/>
+      <c r="H13" s="10"/>
+    </row>
+    <row r="14" spans="1:10">
+      <c r="A14" s="10"/>
+      <c r="B14" s="10"/>
+      <c r="D14" s="10"/>
+      <c r="F14" s="10"/>
+      <c r="H14" s="10"/>
+    </row>
+    <row r="15" spans="1:10">
+      <c r="A15" s="10"/>
+      <c r="B15" s="10"/>
+      <c r="D15" s="10"/>
+      <c r="F15" s="10"/>
+      <c r="H15" s="10"/>
+    </row>
+    <row r="16" spans="1:10">
+      <c r="A16" s="10"/>
+      <c r="B16" s="10"/>
+      <c r="C16" s="10"/>
+      <c r="D16" s="10"/>
+      <c r="F16" s="11"/>
+      <c r="H16" s="11"/>
+      <c r="J16" s="11"/>
+    </row>
+    <row r="17" spans="6:10">
+      <c r="F17" s="11"/>
+      <c r="H17" s="11"/>
+      <c r="J17" s="11"/>
+    </row>
+    <row r="18" spans="6:10">
+      <c r="F18" s="11"/>
+      <c r="H18" s="11"/>
+      <c r="J18" s="11"/>
+    </row>
+    <row r="19" spans="6:10">
+      <c r="F19" s="11"/>
+      <c r="H19" s="11"/>
+      <c r="J19" s="11"/>
+    </row>
+    <row r="20" spans="6:10">
+      <c r="F20" s="11"/>
+      <c r="H20" s="11"/>
+      <c r="J20" s="11"/>
+    </row>
+    <row r="21" spans="6:10">
+      <c r="F21" s="11"/>
+      <c r="H21" s="11"/>
+      <c r="J21" s="11"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3F7416AC-7687-44D6-A243-726C664FB353}">
+  <dimension ref="A2:H7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:C4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="20"/>
+  <sheetData>
+    <row r="2" spans="1:8" ht="23">
+      <c r="A2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" ht="23">
+      <c r="A3" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="23">
+      <c r="A4" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="23">
+      <c r="A5" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="23">
+      <c r="A6" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" ht="23">
+      <c r="A7" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H7" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E0BDBA20-536E-44A7-A29E-A3776AEA0411}">
+  <dimension ref="A2:I7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:C4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="20"/>
+  <sheetData>
+    <row r="2" spans="1:9" ht="23">
+      <c r="A2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" s="1">
+        <v>1</v>
+      </c>
+      <c r="C2" s="1">
+        <v>6</v>
+      </c>
+      <c r="D2" s="1">
+        <v>3</v>
+      </c>
+      <c r="E2" s="1">
+        <v>8</v>
+      </c>
+      <c r="F2" s="1">
+        <v>2</v>
+      </c>
+      <c r="G2" s="1">
+        <v>5</v>
+      </c>
+      <c r="H2" s="1">
+        <v>4</v>
+      </c>
+      <c r="I2" s="1">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" ht="23">
+      <c r="A3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" s="1">
+        <v>3</v>
+      </c>
+      <c r="C3" s="1">
+        <v>5</v>
+      </c>
+      <c r="D3" s="1">
+        <v>1</v>
+      </c>
+      <c r="E3" s="1">
+        <v>7</v>
+      </c>
+      <c r="F3" s="1">
+        <v>4</v>
+      </c>
+      <c r="G3" s="1">
+        <v>6</v>
+      </c>
+      <c r="H3" s="1">
+        <v>2</v>
+      </c>
+      <c r="I3" s="1">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" ht="23">
+      <c r="A4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" s="1">
+        <v>2</v>
+      </c>
+      <c r="C4" s="1">
+        <v>7</v>
+      </c>
+      <c r="D4" s="1">
+        <v>4</v>
+      </c>
+      <c r="E4" s="1">
+        <v>5</v>
+      </c>
+      <c r="F4" s="1">
+        <v>1</v>
+      </c>
+      <c r="G4" s="1">
+        <v>8</v>
+      </c>
+      <c r="H4" s="1">
+        <v>3</v>
+      </c>
+      <c r="I4" s="1">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" ht="23">
+      <c r="A5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5" s="1">
+        <v>1</v>
+      </c>
+      <c r="C5" s="1">
+        <v>4</v>
+      </c>
+      <c r="D5" s="1">
+        <v>6</v>
+      </c>
+      <c r="E5" s="1">
+        <v>7</v>
+      </c>
+      <c r="F5" s="1">
+        <v>2</v>
+      </c>
+      <c r="G5" s="1">
+        <v>3</v>
+      </c>
+      <c r="H5" s="1">
+        <v>5</v>
+      </c>
+      <c r="I5" s="1">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" ht="23">
+      <c r="A6" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6" s="1">
+        <v>6</v>
+      </c>
+      <c r="C6" s="1">
+        <v>8</v>
+      </c>
+      <c r="D6" s="1">
+        <v>2</v>
+      </c>
+      <c r="E6" s="1">
+        <v>4</v>
+      </c>
+      <c r="F6" s="1">
+        <v>5</v>
+      </c>
+      <c r="G6" s="1">
+        <v>7</v>
+      </c>
+      <c r="H6" s="1">
+        <v>1</v>
+      </c>
+      <c r="I6" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" ht="23">
+      <c r="A7" t="s">
+        <v>13</v>
+      </c>
+      <c r="B7" s="1">
+        <v>3</v>
+      </c>
+      <c r="C7" s="1">
+        <v>4</v>
+      </c>
+      <c r="D7" s="1">
+        <v>1</v>
+      </c>
+      <c r="E7" s="1">
+        <v>2</v>
+      </c>
+      <c r="F7" s="1">
+        <v>7</v>
+      </c>
+      <c r="G7" s="1">
+        <v>8</v>
+      </c>
+      <c r="H7" s="1">
+        <v>5</v>
+      </c>
+      <c r="I7" s="1">
+        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fixed crossover B8 tab in rr_templates
</commit_message>
<xml_diff>
--- a/templates/rr_schedules/rr_templates.xlsx
+++ b/templates/rr_schedules/rr_templates.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\z004ercu\Desktop\python\cornerstone\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\UserData\z004ercu\Documents\coding\cornerstone\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66EB04F6-65E2-4B79-BB2A-D98060665423}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A8DEAF2-1D6F-45FA-A15F-CA8D6180501C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28697" yWindow="-103" windowWidth="29006" windowHeight="15806" firstSheet="9" activeTab="11" xr2:uid="{9E58356C-D73F-FC43-AA9C-FFAB6CC6AEB1}"/>
+    <workbookView xWindow="-103" yWindow="-103" windowWidth="16663" windowHeight="8863" firstSheet="20" activeTab="23" xr2:uid="{9E58356C-D73F-FC43-AA9C-FFAB6CC6AEB1}"/>
   </bookViews>
   <sheets>
     <sheet name="rr_3" sheetId="12" r:id="rId1"/>
@@ -38,7 +38,7 @@
     <sheet name="rr_crossover_A8" sheetId="17" r:id="rId23"/>
     <sheet name="rr_crossover_B8" sheetId="18" r:id="rId24"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -46,8 +46,12 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -55,7 +59,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="8">
   <si>
     <t>A1</t>
   </si>
@@ -79,24 +83,6 @@
   </si>
   <si>
     <t>C2</t>
-  </si>
-  <si>
-    <t>round 1</t>
-  </si>
-  <si>
-    <t>round 2</t>
-  </si>
-  <si>
-    <t>round 3</t>
-  </si>
-  <si>
-    <t>round 4</t>
-  </si>
-  <si>
-    <t>round 5</t>
-  </si>
-  <si>
-    <t>round 6</t>
   </si>
 </sst>
 </file>
@@ -1092,7 +1078,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CE116495-6DF0-4588-934F-2AD0E9350DA3}">
   <dimension ref="A2:H15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E7" sqref="A2:H15"/>
     </sheetView>
   </sheetViews>
@@ -4601,7 +4587,7 @@
   <dimension ref="A2:H7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:C4"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="19.75"/>
@@ -4770,185 +4756,167 @@
 
 <file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E0BDBA20-536E-44A7-A29E-A3776AEA0411}">
-  <dimension ref="A2:I7"/>
+  <dimension ref="A2:H7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:C4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:A1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="19.75"/>
   <sheetData>
-    <row r="2" spans="1:9" ht="23.6">
-      <c r="A2" t="s">
-        <v>8</v>
+    <row r="2" spans="1:8" ht="23.6">
+      <c r="A2" s="1">
+        <v>1</v>
       </c>
       <c r="B2" s="1">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="C2" s="1">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="D2" s="1">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="E2" s="1">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="F2" s="1">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="G2" s="1">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="H2" s="1">
-        <v>4</v>
-      </c>
-      <c r="I2" s="1">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" ht="23.6">
-      <c r="A3" t="s">
-        <v>9</v>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" ht="23.6">
+      <c r="A3" s="1">
+        <v>3</v>
       </c>
       <c r="B3" s="1">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="C3" s="1">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="D3" s="1">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="E3" s="1">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="F3" s="1">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="G3" s="1">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="H3" s="1">
-        <v>2</v>
-      </c>
-      <c r="I3" s="1">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" ht="23.6">
-      <c r="A4" t="s">
-        <v>10</v>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="23.6">
+      <c r="A4" s="1">
+        <v>2</v>
       </c>
       <c r="B4" s="1">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="C4" s="1">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="D4" s="1">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="E4" s="1">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="F4" s="1">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="G4" s="1">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="H4" s="1">
-        <v>3</v>
-      </c>
-      <c r="I4" s="1">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" ht="23.6">
-      <c r="A5" t="s">
-        <v>11</v>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="23.6">
+      <c r="A5" s="1">
+        <v>1</v>
       </c>
       <c r="B5" s="1">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="C5" s="1">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="D5" s="1">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E5" s="1">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="F5" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="G5" s="1">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="H5" s="1">
-        <v>5</v>
-      </c>
-      <c r="I5" s="1">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" ht="23.6">
-      <c r="A6" t="s">
-        <v>12</v>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="23.6">
+      <c r="A6" s="1">
+        <v>6</v>
       </c>
       <c r="B6" s="1">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C6" s="1">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="D6" s="1">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="E6" s="1">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F6" s="1">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="G6" s="1">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="H6" s="1">
-        <v>1</v>
-      </c>
-      <c r="I6" s="1">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" ht="23.6">
-      <c r="A7" t="s">
-        <v>13</v>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" ht="23.6">
+      <c r="A7" s="1">
+        <v>3</v>
       </c>
       <c r="B7" s="1">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C7" s="1">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D7" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E7" s="1">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="F7" s="1">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="G7" s="1">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="H7" s="1">
-        <v>5</v>
-      </c>
-      <c r="I7" s="1">
         <v>6</v>
       </c>
     </row>

</xml_diff>